<commit_message>
new excel file 21.11.24
</commit_message>
<xml_diff>
--- a/URS_Certifications-1.xlsx
+++ b/URS_Certifications-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\сайт\сайт2\Сайт на практику\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{536D7B71-9F59-4136-9F68-B9B312BCC106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B464AB7-930B-4CB5-AB6D-280733683055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5760" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5761" uniqueCount="732">
   <si>
     <t>Название компании</t>
   </si>
@@ -3085,15 +3085,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="E139" sqref="E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
@@ -6222,11 +6222,17 @@
       <c r="C138" s="1">
         <v>5246058666</v>
       </c>
+      <c r="D138" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E138" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="G138" s="2">
+        <v>46709</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>